<commit_message>
plotting script revised, empty last column removed
</commit_message>
<xml_diff>
--- a/plotting_and_statistics_script_with_demo_data/output_files_of_py_script/2025-12-03 08_15_00_TEMP_LOG_demo_data.xlsx
+++ b/plotting_and_statistics_script_with_demo_data/output_files_of_py_script/2025-12-03 08_15_00_TEMP_LOG_demo_data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F203"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,11 +463,6 @@
           <t>TMP2</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -487,7 +482,6 @@
       <c r="E2" t="n">
         <v>25.79</v>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -507,7 +501,6 @@
       <c r="E3" t="n">
         <v>25.68</v>
       </c>
-      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -527,7 +520,6 @@
       <c r="E4" t="n">
         <v>25.5</v>
       </c>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -547,7 +539,6 @@
       <c r="E5" t="n">
         <v>25.34</v>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -567,7 +558,6 @@
       <c r="E6" t="n">
         <v>24.91</v>
       </c>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -587,7 +577,6 @@
       <c r="E7" t="n">
         <v>24.82</v>
       </c>
-      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -607,7 +596,6 @@
       <c r="E8" t="n">
         <v>24.7</v>
       </c>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -627,7 +615,6 @@
       <c r="E9" t="n">
         <v>24.91</v>
       </c>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -647,7 +634,6 @@
       <c r="E10" t="n">
         <v>25.49</v>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -667,7 +653,6 @@
       <c r="E11" t="n">
         <v>26.19</v>
       </c>
-      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -687,7 +672,6 @@
       <c r="E12" t="n">
         <v>26.7</v>
       </c>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -707,7 +691,6 @@
       <c r="E13" t="n">
         <v>26.97</v>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -727,7 +710,6 @@
       <c r="E14" t="n">
         <v>27</v>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -747,7 +729,6 @@
       <c r="E15" t="n">
         <v>26.95</v>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -767,7 +748,6 @@
       <c r="E16" t="n">
         <v>27.07</v>
       </c>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -787,7 +767,6 @@
       <c r="E17" t="n">
         <v>27.27</v>
       </c>
-      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -807,7 +786,6 @@
       <c r="E18" t="n">
         <v>27.37</v>
       </c>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -827,7 +805,6 @@
       <c r="E19" t="n">
         <v>27.54</v>
       </c>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -847,7 +824,6 @@
       <c r="E20" t="n">
         <v>27.54</v>
       </c>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -867,7 +843,6 @@
       <c r="E21" t="n">
         <v>27.35</v>
       </c>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -887,7 +862,6 @@
       <c r="E22" t="n">
         <v>27.18</v>
       </c>
-      <c r="F22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -907,7 +881,6 @@
       <c r="E23" t="n">
         <v>26.95</v>
       </c>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -927,7 +900,6 @@
       <c r="E24" t="n">
         <v>26.73</v>
       </c>
-      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -947,7 +919,6 @@
       <c r="E25" t="n">
         <v>26.54</v>
       </c>
-      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -967,7 +938,6 @@
       <c r="E26" t="n">
         <v>26.35</v>
       </c>
-      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -987,7 +957,6 @@
       <c r="E27" t="n">
         <v>26.16</v>
       </c>
-      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1007,7 +976,6 @@
       <c r="E28" t="n">
         <v>26.04</v>
       </c>
-      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1027,7 +995,6 @@
       <c r="E29" t="n">
         <v>25.91</v>
       </c>
-      <c r="F29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1047,7 +1014,6 @@
       <c r="E30" t="n">
         <v>25.83</v>
       </c>
-      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1067,7 +1033,6 @@
       <c r="E31" t="n">
         <v>25.67</v>
       </c>
-      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1087,7 +1052,6 @@
       <c r="E32" t="n">
         <v>25.55</v>
       </c>
-      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1107,7 +1071,6 @@
       <c r="E33" t="n">
         <v>25.6</v>
       </c>
-      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1127,7 +1090,6 @@
       <c r="E34" t="n">
         <v>26.18</v>
       </c>
-      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1147,7 +1109,6 @@
       <c r="E35" t="n">
         <v>25.74</v>
       </c>
-      <c r="F35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1167,7 +1128,6 @@
       <c r="E36" t="n">
         <v>26.27</v>
       </c>
-      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1187,7 +1147,6 @@
       <c r="E37" t="n">
         <v>27.8</v>
       </c>
-      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1207,7 +1166,6 @@
       <c r="E38" t="n">
         <v>31.52</v>
       </c>
-      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1227,7 +1185,6 @@
       <c r="E39" t="n">
         <v>31.95</v>
       </c>
-      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1247,7 +1204,6 @@
       <c r="E40" t="n">
         <v>31.8</v>
       </c>
-      <c r="F40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1267,7 +1223,6 @@
       <c r="E41" t="n">
         <v>31.41</v>
       </c>
-      <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1287,7 +1242,6 @@
       <c r="E42" t="n">
         <v>31.13</v>
       </c>
-      <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1307,7 +1261,6 @@
       <c r="E43" t="n">
         <v>31.66</v>
       </c>
-      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1327,7 +1280,6 @@
       <c r="E44" t="n">
         <v>31.92</v>
       </c>
-      <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1347,7 +1299,6 @@
       <c r="E45" t="n">
         <v>31.8</v>
       </c>
-      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1367,7 +1318,6 @@
       <c r="E46" t="n">
         <v>31.38</v>
       </c>
-      <c r="F46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1387,7 +1337,6 @@
       <c r="E47" t="n">
         <v>31.05</v>
       </c>
-      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1407,7 +1356,6 @@
       <c r="E48" t="n">
         <v>30.54</v>
       </c>
-      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1427,7 +1375,6 @@
       <c r="E49" t="n">
         <v>30.2</v>
       </c>
-      <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1447,7 +1394,6 @@
       <c r="E50" t="n">
         <v>29.8</v>
       </c>
-      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1467,7 +1413,6 @@
       <c r="E51" t="n">
         <v>29.4</v>
       </c>
-      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1487,7 +1432,6 @@
       <c r="E52" t="n">
         <v>29.09</v>
       </c>
-      <c r="F52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1507,7 +1451,6 @@
       <c r="E53" t="n">
         <v>28.69</v>
       </c>
-      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1527,7 +1470,6 @@
       <c r="E54" t="n">
         <v>28.36</v>
       </c>
-      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1547,7 +1489,6 @@
       <c r="E55" t="n">
         <v>28.01</v>
       </c>
-      <c r="F55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1567,7 +1508,6 @@
       <c r="E56" t="n">
         <v>27.73</v>
       </c>
-      <c r="F56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1587,7 +1527,6 @@
       <c r="E57" t="n">
         <v>27.42</v>
       </c>
-      <c r="F57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1607,7 +1546,6 @@
       <c r="E58" t="n">
         <v>27.14</v>
       </c>
-      <c r="F58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1627,7 +1565,6 @@
       <c r="E59" t="n">
         <v>26.88</v>
       </c>
-      <c r="F59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1647,7 +1584,6 @@
       <c r="E60" t="n">
         <v>26.63</v>
       </c>
-      <c r="F60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1667,7 +1603,6 @@
       <c r="E61" t="n">
         <v>26.38</v>
       </c>
-      <c r="F61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1687,7 +1622,6 @@
       <c r="E62" t="n">
         <v>26.17</v>
       </c>
-      <c r="F62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1707,7 +1641,6 @@
       <c r="E63" t="n">
         <v>25.99</v>
       </c>
-      <c r="F63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1727,7 +1660,6 @@
       <c r="E64" t="n">
         <v>25.8</v>
       </c>
-      <c r="F64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1747,7 +1679,6 @@
       <c r="E65" t="n">
         <v>25.64</v>
       </c>
-      <c r="F65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1767,7 +1698,6 @@
       <c r="E66" t="n">
         <v>25.49</v>
       </c>
-      <c r="F66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1787,7 +1717,6 @@
       <c r="E67" t="n">
         <v>25.7</v>
       </c>
-      <c r="F67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1807,7 +1736,6 @@
       <c r="E68" t="n">
         <v>27.16</v>
       </c>
-      <c r="F68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1827,7 +1755,6 @@
       <c r="E69" t="n">
         <v>27.73</v>
       </c>
-      <c r="F69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1847,7 +1774,6 @@
       <c r="E70" t="n">
         <v>27.68</v>
       </c>
-      <c r="F70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1867,7 +1793,6 @@
       <c r="E71" t="n">
         <v>27.43</v>
       </c>
-      <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1887,7 +1812,6 @@
       <c r="E72" t="n">
         <v>27.19</v>
       </c>
-      <c r="F72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1907,7 +1831,6 @@
       <c r="E73" t="n">
         <v>26.84</v>
       </c>
-      <c r="F73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1927,7 +1850,6 @@
       <c r="E74" t="n">
         <v>26.57</v>
       </c>
-      <c r="F74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1947,7 +1869,6 @@
       <c r="E75" t="n">
         <v>26.28</v>
       </c>
-      <c r="F75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1967,7 +1888,6 @@
       <c r="E76" t="n">
         <v>26.03</v>
       </c>
-      <c r="F76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1987,7 +1907,6 @@
       <c r="E77" t="n">
         <v>25.81</v>
       </c>
-      <c r="F77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2007,7 +1926,6 @@
       <c r="E78" t="n">
         <v>25.57</v>
       </c>
-      <c r="F78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2027,7 +1945,6 @@
       <c r="E79" t="n">
         <v>25.36</v>
       </c>
-      <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2047,7 +1964,6 @@
       <c r="E80" t="n">
         <v>25.13</v>
       </c>
-      <c r="F80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2067,7 +1983,6 @@
       <c r="E81" t="n">
         <v>24.91</v>
       </c>
-      <c r="F81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2087,7 +2002,6 @@
       <c r="E82" t="n">
         <v>24.76</v>
       </c>
-      <c r="F82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2107,7 +2021,6 @@
       <c r="E83" t="n">
         <v>24.54</v>
       </c>
-      <c r="F83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2127,7 +2040,6 @@
       <c r="E84" t="n">
         <v>24.43</v>
       </c>
-      <c r="F84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2147,7 +2059,6 @@
       <c r="E85" t="n">
         <v>24.25</v>
       </c>
-      <c r="F85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2167,7 +2078,6 @@
       <c r="E86" t="n">
         <v>24.11</v>
       </c>
-      <c r="F86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2187,7 +2097,6 @@
       <c r="E87" t="n">
         <v>23.94</v>
       </c>
-      <c r="F87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2207,7 +2116,6 @@
       <c r="E88" t="n">
         <v>23.81</v>
       </c>
-      <c r="F88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2227,7 +2135,6 @@
       <c r="E89" t="n">
         <v>23.7</v>
       </c>
-      <c r="F89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2247,7 +2154,6 @@
       <c r="E90" t="n">
         <v>23.56</v>
       </c>
-      <c r="F90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2267,7 +2173,6 @@
       <c r="E91" t="n">
         <v>23.42</v>
       </c>
-      <c r="F91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2287,7 +2192,6 @@
       <c r="E92" t="n">
         <v>23.31</v>
       </c>
-      <c r="F92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2307,7 +2211,6 @@
       <c r="E93" t="n">
         <v>23.21</v>
       </c>
-      <c r="F93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2327,7 +2230,6 @@
       <c r="E94" t="n">
         <v>23.11</v>
       </c>
-      <c r="F94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2347,7 +2249,6 @@
       <c r="E95" t="n">
         <v>23.05</v>
       </c>
-      <c r="F95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2367,7 +2268,6 @@
       <c r="E96" t="n">
         <v>22.99</v>
       </c>
-      <c r="F96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2387,7 +2287,6 @@
       <c r="E97" t="n">
         <v>22.84</v>
       </c>
-      <c r="F97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2407,7 +2306,6 @@
       <c r="E98" t="n">
         <v>22.84</v>
       </c>
-      <c r="F98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2427,7 +2325,6 @@
       <c r="E99" t="n">
         <v>22.78</v>
       </c>
-      <c r="F99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2447,7 +2344,6 @@
       <c r="E100" t="n">
         <v>22.7</v>
       </c>
-      <c r="F100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2467,7 +2363,6 @@
       <c r="E101" t="n">
         <v>22.6</v>
       </c>
-      <c r="F101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2487,7 +2382,6 @@
       <c r="E102" t="n">
         <v>22.52</v>
       </c>
-      <c r="F102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2507,7 +2401,6 @@
       <c r="E103" t="n">
         <v>22.44</v>
       </c>
-      <c r="F103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2527,7 +2420,6 @@
       <c r="E104" t="n">
         <v>22.34</v>
       </c>
-      <c r="F104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2547,7 +2439,6 @@
       <c r="E105" t="n">
         <v>22.3</v>
       </c>
-      <c r="F105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2567,7 +2458,6 @@
       <c r="E106" t="n">
         <v>22.23</v>
       </c>
-      <c r="F106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2587,7 +2477,6 @@
       <c r="E107" t="n">
         <v>22.14</v>
       </c>
-      <c r="F107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2607,7 +2496,6 @@
       <c r="E108" t="n">
         <v>22.08</v>
       </c>
-      <c r="F108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2627,7 +2515,6 @@
       <c r="E109" t="n">
         <v>22.03</v>
       </c>
-      <c r="F109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2647,7 +2534,6 @@
       <c r="E110" t="n">
         <v>21.98</v>
       </c>
-      <c r="F110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2667,7 +2553,6 @@
       <c r="E111" t="n">
         <v>21.9</v>
       </c>
-      <c r="F111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2687,7 +2572,6 @@
       <c r="E112" t="n">
         <v>21.87</v>
       </c>
-      <c r="F112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2707,7 +2591,6 @@
       <c r="E113" t="n">
         <v>21.8</v>
       </c>
-      <c r="F113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2727,7 +2610,6 @@
       <c r="E114" t="n">
         <v>21.75</v>
       </c>
-      <c r="F114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2747,7 +2629,6 @@
       <c r="E115" t="n">
         <v>21.71</v>
       </c>
-      <c r="F115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2767,7 +2648,6 @@
       <c r="E116" t="n">
         <v>21.67</v>
       </c>
-      <c r="F116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2787,7 +2667,6 @@
       <c r="E117" t="n">
         <v>21.62</v>
       </c>
-      <c r="F117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2807,7 +2686,6 @@
       <c r="E118" t="n">
         <v>21.55</v>
       </c>
-      <c r="F118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2827,7 +2705,6 @@
       <c r="E119" t="n">
         <v>21.52</v>
       </c>
-      <c r="F119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2847,7 +2724,6 @@
       <c r="E120" t="n">
         <v>21.48</v>
       </c>
-      <c r="F120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2867,7 +2743,6 @@
       <c r="E121" t="n">
         <v>21.44</v>
       </c>
-      <c r="F121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2887,7 +2762,6 @@
       <c r="E122" t="n">
         <v>21.39</v>
       </c>
-      <c r="F122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2907,7 +2781,6 @@
       <c r="E123" t="n">
         <v>21.37</v>
       </c>
-      <c r="F123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2927,7 +2800,6 @@
       <c r="E124" t="n">
         <v>21.32</v>
       </c>
-      <c r="F124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2947,7 +2819,6 @@
       <c r="E125" t="n">
         <v>21.3</v>
       </c>
-      <c r="F125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2967,7 +2838,6 @@
       <c r="E126" t="n">
         <v>21.25</v>
       </c>
-      <c r="F126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2987,7 +2857,6 @@
       <c r="E127" t="n">
         <v>21.23</v>
       </c>
-      <c r="F127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -3007,7 +2876,6 @@
       <c r="E128" t="n">
         <v>21.2</v>
       </c>
-      <c r="F128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -3027,7 +2895,6 @@
       <c r="E129" t="n">
         <v>21.17</v>
       </c>
-      <c r="F129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -3047,7 +2914,6 @@
       <c r="E130" t="n">
         <v>21.14</v>
       </c>
-      <c r="F130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -3067,7 +2933,6 @@
       <c r="E131" t="n">
         <v>21.11</v>
       </c>
-      <c r="F131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -3087,7 +2952,6 @@
       <c r="E132" t="n">
         <v>21.07</v>
       </c>
-      <c r="F132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -3107,7 +2971,6 @@
       <c r="E133" t="n">
         <v>21.05</v>
       </c>
-      <c r="F133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -3127,7 +2990,6 @@
       <c r="E134" t="n">
         <v>21.03</v>
       </c>
-      <c r="F134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3147,7 +3009,6 @@
       <c r="E135" t="n">
         <v>20.99</v>
       </c>
-      <c r="F135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3167,7 +3028,6 @@
       <c r="E136" t="n">
         <v>20.98</v>
       </c>
-      <c r="F136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3187,7 +3047,6 @@
       <c r="E137" t="n">
         <v>20.95</v>
       </c>
-      <c r="F137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3207,7 +3066,6 @@
       <c r="E138" t="n">
         <v>20.92</v>
       </c>
-      <c r="F138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3227,7 +3085,6 @@
       <c r="E139" t="n">
         <v>20.88</v>
       </c>
-      <c r="F139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3247,7 +3104,6 @@
       <c r="E140" t="n">
         <v>20.86</v>
       </c>
-      <c r="F140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3267,7 +3123,6 @@
       <c r="E141" t="n">
         <v>20.84</v>
       </c>
-      <c r="F141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3287,7 +3142,6 @@
       <c r="E142" t="n">
         <v>20.8</v>
       </c>
-      <c r="F142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3307,7 +3161,6 @@
       <c r="E143" t="n">
         <v>20.77</v>
       </c>
-      <c r="F143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3327,7 +3180,6 @@
       <c r="E144" t="n">
         <v>20.73</v>
       </c>
-      <c r="F144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3347,7 +3199,6 @@
       <c r="E145" t="n">
         <v>20.73</v>
       </c>
-      <c r="F145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3367,7 +3218,6 @@
       <c r="E146" t="n">
         <v>20.68</v>
       </c>
-      <c r="F146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3387,7 +3237,6 @@
       <c r="E147" t="n">
         <v>20.64</v>
       </c>
-      <c r="F147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -3407,7 +3256,6 @@
       <c r="E148" t="n">
         <v>20.63</v>
       </c>
-      <c r="F148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3427,7 +3275,6 @@
       <c r="E149" t="n">
         <v>20.59</v>
       </c>
-      <c r="F149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -3447,7 +3294,6 @@
       <c r="E150" t="n">
         <v>20.59</v>
       </c>
-      <c r="F150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -3467,7 +3313,6 @@
       <c r="E151" t="n">
         <v>20.55</v>
       </c>
-      <c r="F151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3487,7 +3332,6 @@
       <c r="E152" t="n">
         <v>20.52</v>
       </c>
-      <c r="F152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3507,7 +3351,6 @@
       <c r="E153" t="n">
         <v>20.5</v>
       </c>
-      <c r="F153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3527,7 +3370,6 @@
       <c r="E154" t="n">
         <v>20.48</v>
       </c>
-      <c r="F154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3547,7 +3389,6 @@
       <c r="E155" t="n">
         <v>20.46</v>
       </c>
-      <c r="F155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3567,7 +3408,6 @@
       <c r="E156" t="n">
         <v>20.45</v>
       </c>
-      <c r="F156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3587,7 +3427,6 @@
       <c r="E157" t="n">
         <v>20.42</v>
       </c>
-      <c r="F157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3607,7 +3446,6 @@
       <c r="E158" t="n">
         <v>20.41</v>
       </c>
-      <c r="F158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3627,7 +3465,6 @@
       <c r="E159" t="n">
         <v>20.38</v>
       </c>
-      <c r="F159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3647,7 +3484,6 @@
       <c r="E160" t="n">
         <v>20.37</v>
       </c>
-      <c r="F160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3667,7 +3503,6 @@
       <c r="E161" t="n">
         <v>20.34</v>
       </c>
-      <c r="F161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -3687,7 +3522,6 @@
       <c r="E162" t="n">
         <v>20.33</v>
       </c>
-      <c r="F162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -3707,7 +3541,6 @@
       <c r="E163" t="n">
         <v>20.32</v>
       </c>
-      <c r="F163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -3727,7 +3560,6 @@
       <c r="E164" t="n">
         <v>20.3</v>
       </c>
-      <c r="F164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -3747,7 +3579,6 @@
       <c r="E165" t="n">
         <v>27.02</v>
       </c>
-      <c r="F165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -3767,7 +3598,6 @@
       <c r="E166" t="n">
         <v>31.09</v>
       </c>
-      <c r="F166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -3787,7 +3617,6 @@
       <c r="E167" t="n">
         <v>33.21</v>
       </c>
-      <c r="F167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -3807,7 +3636,6 @@
       <c r="E168" t="n">
         <v>33.96</v>
       </c>
-      <c r="F168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3827,7 +3655,6 @@
       <c r="E169" t="n">
         <v>34.02</v>
       </c>
-      <c r="F169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -3847,7 +3674,6 @@
       <c r="E170" t="n">
         <v>33.74</v>
       </c>
-      <c r="F170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3867,7 +3693,6 @@
       <c r="E171" t="n">
         <v>33.22</v>
       </c>
-      <c r="F171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -3887,7 +3712,6 @@
       <c r="E172" t="n">
         <v>32.57</v>
       </c>
-      <c r="F172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -3907,7 +3731,6 @@
       <c r="E173" t="n">
         <v>31.99</v>
       </c>
-      <c r="F173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3927,7 +3750,6 @@
       <c r="E174" t="n">
         <v>31.4</v>
       </c>
-      <c r="F174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3947,7 +3769,6 @@
       <c r="E175" t="n">
         <v>30.81</v>
       </c>
-      <c r="F175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3967,7 +3788,6 @@
       <c r="E176" t="n">
         <v>30.22</v>
       </c>
-      <c r="F176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3987,7 +3807,6 @@
       <c r="E177" t="n">
         <v>29.68</v>
       </c>
-      <c r="F177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -4007,7 +3826,6 @@
       <c r="E178" t="n">
         <v>29.23</v>
       </c>
-      <c r="F178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -4027,7 +3845,6 @@
       <c r="E179" t="n">
         <v>28.75</v>
       </c>
-      <c r="F179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -4047,7 +3864,6 @@
       <c r="E180" t="n">
         <v>28.32</v>
       </c>
-      <c r="F180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -4067,7 +3883,6 @@
       <c r="E181" t="n">
         <v>27.91</v>
       </c>
-      <c r="F181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -4087,7 +3902,6 @@
       <c r="E182" t="n">
         <v>27.49</v>
       </c>
-      <c r="F182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -4107,7 +3921,6 @@
       <c r="E183" t="n">
         <v>27.16</v>
       </c>
-      <c r="F183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -4127,7 +3940,6 @@
       <c r="E184" t="n">
         <v>26.79</v>
       </c>
-      <c r="F184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -4147,7 +3959,6 @@
       <c r="E185" t="n">
         <v>26.48</v>
       </c>
-      <c r="F185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -4167,7 +3978,6 @@
       <c r="E186" t="n">
         <v>26.18</v>
       </c>
-      <c r="F186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -4187,7 +3997,6 @@
       <c r="E187" t="n">
         <v>25.88</v>
       </c>
-      <c r="F187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4207,7 +4016,6 @@
       <c r="E188" t="n">
         <v>25.61</v>
       </c>
-      <c r="F188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4227,7 +4035,6 @@
       <c r="E189" t="n">
         <v>25.4</v>
       </c>
-      <c r="F189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4247,7 +4054,6 @@
       <c r="E190" t="n">
         <v>25.16</v>
       </c>
-      <c r="F190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4267,7 +4073,6 @@
       <c r="E191" t="n">
         <v>24.88</v>
       </c>
-      <c r="F191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4287,7 +4092,6 @@
       <c r="E192" t="n">
         <v>21.53</v>
       </c>
-      <c r="F192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4307,7 +4111,6 @@
       <c r="E193" t="n">
         <v>23.73</v>
       </c>
-      <c r="F193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4327,7 +4130,6 @@
       <c r="E194" t="n">
         <v>24.02</v>
       </c>
-      <c r="F194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4347,7 +4149,6 @@
       <c r="E195" t="n">
         <v>30.24</v>
       </c>
-      <c r="F195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4367,7 +4168,6 @@
       <c r="E196" t="n">
         <v>34.13</v>
       </c>
-      <c r="F196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4387,7 +4187,6 @@
       <c r="E197" t="n">
         <v>34.83</v>
       </c>
-      <c r="F197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -4407,7 +4206,6 @@
       <c r="E198" t="n">
         <v>34.88</v>
       </c>
-      <c r="F198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -4427,7 +4225,6 @@
       <c r="E199" t="n">
         <v>34.42</v>
       </c>
-      <c r="F199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -4447,7 +4244,6 @@
       <c r="E200" t="n">
         <v>33.73</v>
       </c>
-      <c r="F200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -4467,7 +4263,6 @@
       <c r="E201" t="n">
         <v>33.02</v>
       </c>
-      <c r="F201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -4487,7 +4282,6 @@
       <c r="E202" t="n">
         <v>32.17</v>
       </c>
-      <c r="F202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -4507,7 +4301,6 @@
       <c r="E203" t="n">
         <v>31.55</v>
       </c>
-      <c r="F203" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>